<commit_message>
Add CLI runner for SQL scripts
</commit_message>
<xml_diff>
--- a/4.Project_Files/Data Insight.xlsx
+++ b/4.Project_Files/Data Insight.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthqld.sharepoint.com/sites/CSD-AccountsPayable/Reporting/A001_Data_Analytics/A0017_PIOR/4. Project_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthqld.sharepoint.com/sites/CSD-AccountsPayable/Reporting/A001_Data_Analytics/A0017_PIOR/4.Project_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="844" documentId="8_{044127FF-EB8D-45C1-B97C-105321731508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F031EB65-F90D-49A6-B9A1-CAA5043BBCA4}"/>
+  <xr:revisionPtr revIDLastSave="845" documentId="8_{044127FF-EB8D-45C1-B97C-105321731508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCDEFCF3-5884-4E2C-B28C-4C7CFE25FF5C}"/>
   <bookViews>
-    <workbookView xWindow="-51720" yWindow="210" windowWidth="51840" windowHeight="21120" tabRatio="859" firstSheet="1" activeTab="5" xr2:uid="{3B62FA93-2D3E-4B50-B6E4-AB4E7E76766D}"/>
+    <workbookView minimized="1" xWindow="-50475" yWindow="1455" windowWidth="38700" windowHeight="15345" tabRatio="859" firstSheet="1" activeTab="5" xr2:uid="{3B62FA93-2D3E-4B50-B6E4-AB4E7E76766D}"/>
   </bookViews>
   <sheets>
     <sheet name="Key Findings" sheetId="9" r:id="rId1"/>
@@ -2357,7 +2357,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A27"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="101.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,7 +2402,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>98</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>101</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>103</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>106</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>108</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>110</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>112</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>114</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>118</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>120</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>122</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>124</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>126</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>128</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>130</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>132</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>134</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>136</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>138</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>140</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>142</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>147</v>
       </c>
@@ -2771,7 +2771,7 @@
   <autoFilter ref="A2:C36" xr:uid="{E005D97C-7DD0-49FB-98DF-245E46BF6FCA}">
     <filterColumn colId="1">
       <filters>
-        <filter val="VIM_1HEAD_2HEAD_VW"/>
+        <filter val="VIM_STG_T101T_VW"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>